<commit_message>
database merge into single csv
</commit_message>
<xml_diff>
--- a/Columnas.xlsx
+++ b/Columnas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alevi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\DataMining_Proyect1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BB899E-FF5D-4016-A734-2431FACD0783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F70D9F-8124-45B8-ABFD-B8030A4F9C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="1005" windowWidth="24240" windowHeight="12420" xr2:uid="{A1FDD086-864A-413C-8FCA-D99F4E992385}"/>
+    <workbookView xWindow="3345" yWindow="2385" windowWidth="24240" windowHeight="12420" xr2:uid="{A1FDD086-864A-413C-8FCA-D99F4E992385}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="73">
   <si>
     <t>Depreg</t>
   </si>
@@ -239,6 +239,21 @@
   </si>
   <si>
     <t>Año de ocurrencia</t>
+  </si>
+  <si>
+    <t>Pueblo de pertenencia de la Madre</t>
+  </si>
+  <si>
+    <t>Ocupación (Subgrupos CIUO-08) de la madre</t>
+  </si>
+  <si>
+    <t>GRETNM</t>
+  </si>
+  <si>
+    <t>OCUPAM</t>
+  </si>
+  <si>
+    <t>NACIONM</t>
   </si>
 </sst>
 </file>
@@ -271,7 +286,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,6 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -633,17 +649,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3283B29-4A7A-493D-87FA-0FC2E01C9DCE}">
-  <dimension ref="A1:AG42"/>
+  <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -701,14 +718,14 @@
       <c r="Q2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="6"/>
+      <c r="R2" s="7"/>
       <c r="S2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="6"/>
+      <c r="U2" s="7"/>
       <c r="V2" s="5" t="s">
         <v>18</v>
       </c>
@@ -721,7 +738,7 @@
       <c r="Y2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="6"/>
+      <c r="Z2" s="7"/>
       <c r="AA2" s="5" t="s">
         <v>22</v>
       </c>
@@ -796,14 +813,14 @@
       <c r="Q3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="6"/>
+      <c r="R3" s="7"/>
       <c r="S3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="6"/>
+      <c r="U3" s="7"/>
       <c r="V3" s="5" t="s">
         <v>18</v>
       </c>
@@ -816,7 +833,7 @@
       <c r="Y3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="Z3" s="6"/>
+      <c r="Z3" s="7"/>
       <c r="AA3" s="5" t="s">
         <v>22</v>
       </c>
@@ -853,51 +870,51 @@
         <v>31</v>
       </c>
       <c r="E4" s="5" t="str">
-        <f>UPPER(E3)</f>
+        <f t="shared" ref="E4:E11" si="0">UPPER(E3)</f>
         <v>AÑOREG</v>
       </c>
       <c r="F4" s="5" t="str">
-        <f t="shared" ref="F4:H4" si="0">UPPER(F3)</f>
+        <f t="shared" ref="F4:H4" si="1">UPPER(F3)</f>
         <v>DEPOCU</v>
       </c>
       <c r="G4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>MUPOCU</v>
       </c>
       <c r="H4" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>AREAG</v>
       </c>
       <c r="I4" s="5" t="str">
-        <f t="shared" ref="I4" si="1">UPPER(I3)</f>
+        <f t="shared" ref="I4" si="2">UPPER(I3)</f>
         <v>SEXO</v>
       </c>
       <c r="J4" s="5" t="str">
-        <f t="shared" ref="J4" si="2">UPPER(J3)</f>
+        <f t="shared" ref="J4" si="3">UPPER(J3)</f>
         <v>DIAOCU</v>
       </c>
       <c r="K4" s="5" t="str">
-        <f t="shared" ref="K4" si="3">UPPER(K3)</f>
+        <f t="shared" ref="K4" si="4">UPPER(K3)</f>
         <v>MESOCU</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="7"/>
       <c r="M4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="5" t="str">
-        <f>UPPER(N3)</f>
+        <f t="shared" ref="N4:N11" si="5">UPPER(N3)</f>
         <v>CLAPAR</v>
       </c>
       <c r="O4" s="5" t="str">
-        <f t="shared" ref="O4:Q4" si="4">UPPER(O3)</f>
+        <f t="shared" ref="O4:Q4" si="6">UPPER(O3)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P4" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>SEMGES</v>
       </c>
       <c r="Q4" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>EDADM</v>
       </c>
       <c r="R4" s="5" t="s">
@@ -908,53 +925,51 @@
         <v>DEPREM</v>
       </c>
       <c r="T4" s="5" t="str">
-        <f t="shared" ref="T4:W6" si="5">UPPER(T3)</f>
+        <f t="shared" ref="T4:W6" si="7">UPPER(T3)</f>
         <v>MUPREM</v>
       </c>
-      <c r="U4" s="6"/>
-      <c r="V4" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>GRETNM</v>
+      <c r="U4" s="7"/>
+      <c r="V4" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="W4" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>ESCIVM</v>
       </c>
       <c r="X4" s="5" t="str">
-        <f t="shared" ref="X4" si="6">UPPER(X3)</f>
+        <f t="shared" ref="X4" si="8">UPPER(X3)</f>
         <v>NACIOM</v>
       </c>
       <c r="Y4" s="5" t="str">
-        <f t="shared" ref="Y4" si="7">UPPER(Y3)</f>
+        <f t="shared" ref="Y4" si="9">UPPER(Y3)</f>
         <v>ESCOLAM</v>
       </c>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="5" t="str">
-        <f t="shared" ref="AA4" si="8">UPPER(AA3)</f>
-        <v>OCUPAM</v>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="AB4" s="5" t="str">
-        <f t="shared" ref="AB4" si="9">UPPER(AB3)</f>
+        <f t="shared" ref="AB4" si="10">UPPER(AB3)</f>
         <v>CAUDEF</v>
       </c>
       <c r="AC4" s="5" t="str">
-        <f t="shared" ref="AC4" si="10">UPPER(AC3)</f>
+        <f t="shared" ref="AC4" si="11">UPPER(AC3)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD4" s="5" t="str">
-        <f t="shared" ref="AD4" si="11">UPPER(AD3)</f>
+        <f t="shared" ref="AD4" si="12">UPPER(AD3)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE4" s="5" t="str">
-        <f t="shared" ref="AE4" si="12">UPPER(AE3)</f>
+        <f t="shared" ref="AE4" si="13">UPPER(AE3)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF4" s="5" t="str">
-        <f t="shared" ref="AF4" si="13">UPPER(AF3)</f>
+        <f t="shared" ref="AF4" si="14">UPPER(AF3)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG4" s="5" t="str">
-        <f t="shared" ref="AG4" si="14">UPPER(AG3)</f>
+        <f t="shared" ref="AG4" si="15">UPPER(AG3)</f>
         <v>TOHIVI</v>
       </c>
     </row>
@@ -972,51 +987,51 @@
         <v>31</v>
       </c>
       <c r="E5" s="5" t="str">
-        <f>UPPER(E4)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F5" s="5" t="str">
-        <f t="shared" ref="F5" si="15">UPPER(F4)</f>
+        <f t="shared" ref="F5" si="16">UPPER(F4)</f>
         <v>DEPOCU</v>
       </c>
       <c r="G5" s="5" t="str">
-        <f t="shared" ref="G5" si="16">UPPER(G4)</f>
+        <f t="shared" ref="G5" si="17">UPPER(G4)</f>
         <v>MUPOCU</v>
       </c>
       <c r="H5" s="5" t="str">
-        <f t="shared" ref="H5" si="17">UPPER(H4)</f>
+        <f t="shared" ref="H5" si="18">UPPER(H4)</f>
         <v>AREAG</v>
       </c>
       <c r="I5" s="5" t="str">
-        <f t="shared" ref="I5" si="18">UPPER(I4)</f>
+        <f t="shared" ref="I5" si="19">UPPER(I4)</f>
         <v>SEXO</v>
       </c>
       <c r="J5" s="5" t="str">
-        <f t="shared" ref="J5" si="19">UPPER(J4)</f>
+        <f t="shared" ref="J5" si="20">UPPER(J4)</f>
         <v>DIAOCU</v>
       </c>
       <c r="K5" s="5" t="str">
-        <f t="shared" ref="K5" si="20">UPPER(K4)</f>
+        <f t="shared" ref="K5" si="21">UPPER(K4)</f>
         <v>MESOCU</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="7"/>
       <c r="M5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="5" t="str">
-        <f>UPPER(N4)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O5" s="5" t="str">
-        <f t="shared" ref="O5" si="21">UPPER(O4)</f>
+        <f t="shared" ref="O5" si="22">UPPER(O4)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P5" s="5" t="str">
-        <f t="shared" ref="P5" si="22">UPPER(P4)</f>
+        <f t="shared" ref="P5" si="23">UPPER(P4)</f>
         <v>SEMGES</v>
       </c>
       <c r="Q5" s="5" t="str">
-        <f t="shared" ref="Q5" si="23">UPPER(Q4)</f>
+        <f t="shared" ref="Q5" si="24">UPPER(Q4)</f>
         <v>EDADM</v>
       </c>
       <c r="R5" s="5" t="s">
@@ -1027,51 +1042,51 @@
         <v>DEPREM</v>
       </c>
       <c r="T5" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>MUPREM</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="6"/>
+      <c r="V5" s="7"/>
       <c r="W5" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>ESCIVM</v>
       </c>
       <c r="X5" s="5" t="str">
-        <f t="shared" ref="X5" si="24">UPPER(X4)</f>
+        <f t="shared" ref="X5" si="25">UPPER(X4)</f>
         <v>NACIOM</v>
       </c>
       <c r="Y5" s="5" t="str">
-        <f t="shared" ref="Y5" si="25">UPPER(Y4)</f>
+        <f t="shared" ref="Y5" si="26">UPPER(Y4)</f>
         <v>ESCOLAM</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA5" s="6"/>
+      <c r="AA5" s="7"/>
       <c r="AB5" s="5" t="str">
-        <f t="shared" ref="AB5:AB6" si="26">UPPER(AB4)</f>
+        <f t="shared" ref="AB5:AB6" si="27">UPPER(AB4)</f>
         <v>CAUDEF</v>
       </c>
       <c r="AC5" s="5" t="str">
-        <f t="shared" ref="AC5" si="27">UPPER(AC4)</f>
+        <f t="shared" ref="AC5" si="28">UPPER(AC4)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD5" s="5" t="str">
-        <f t="shared" ref="AD5" si="28">UPPER(AD4)</f>
+        <f t="shared" ref="AD5" si="29">UPPER(AD4)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE5" s="5" t="str">
-        <f t="shared" ref="AE5" si="29">UPPER(AE4)</f>
+        <f t="shared" ref="AE5" si="30">UPPER(AE4)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF5" s="5" t="str">
-        <f t="shared" ref="AF5" si="30">UPPER(AF4)</f>
+        <f t="shared" ref="AF5" si="31">UPPER(AF4)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG5" s="5" t="str">
-        <f t="shared" ref="AG5" si="31">UPPER(AG4)</f>
+        <f t="shared" ref="AG5" si="32">UPPER(AG4)</f>
         <v>TOHIVI</v>
       </c>
     </row>
@@ -1089,51 +1104,51 @@
         <v>31</v>
       </c>
       <c r="E6" s="5" t="str">
-        <f>UPPER(E5)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F6" s="5" t="str">
-        <f>UPPER(F5)</f>
+        <f t="shared" ref="F6:F11" si="33">UPPER(F5)</f>
         <v>DEPOCU</v>
       </c>
       <c r="G6" s="5" t="str">
-        <f t="shared" ref="G6" si="32">UPPER(G5)</f>
+        <f t="shared" ref="G6" si="34">UPPER(G5)</f>
         <v>MUPOCU</v>
       </c>
       <c r="H6" s="5" t="str">
-        <f t="shared" ref="H6" si="33">UPPER(H5)</f>
+        <f t="shared" ref="H6" si="35">UPPER(H5)</f>
         <v>AREAG</v>
       </c>
       <c r="I6" s="5" t="str">
-        <f t="shared" ref="I6" si="34">UPPER(I5)</f>
+        <f t="shared" ref="I6" si="36">UPPER(I5)</f>
         <v>SEXO</v>
       </c>
       <c r="J6" s="5" t="str">
-        <f t="shared" ref="J6" si="35">UPPER(J5)</f>
+        <f t="shared" ref="J6" si="37">UPPER(J5)</f>
         <v>DIAOCU</v>
       </c>
       <c r="K6" s="5" t="str">
-        <f t="shared" ref="K6" si="36">UPPER(K5)</f>
+        <f t="shared" ref="K6" si="38">UPPER(K5)</f>
         <v>MESOCU</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="7"/>
       <c r="M6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N6" s="5" t="str">
-        <f>UPPER(N5)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O6" s="5" t="str">
-        <f t="shared" ref="O6" si="37">UPPER(O5)</f>
+        <f t="shared" ref="O6" si="39">UPPER(O5)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P6" s="5" t="str">
-        <f t="shared" ref="P6" si="38">UPPER(P5)</f>
+        <f t="shared" ref="P6" si="40">UPPER(P5)</f>
         <v>SEMGES</v>
       </c>
       <c r="Q6" s="5" t="str">
-        <f t="shared" ref="Q6" si="39">UPPER(Q5)</f>
+        <f t="shared" ref="Q6" si="41">UPPER(Q5)</f>
         <v>EDADM</v>
       </c>
       <c r="R6" s="5" t="s">
@@ -1144,51 +1159,51 @@
         <v>DEPREM</v>
       </c>
       <c r="T6" s="5" t="str">
-        <f t="shared" ref="T6" si="40">UPPER(T5)</f>
+        <f t="shared" ref="T6" si="42">UPPER(T5)</f>
         <v>MUPREM</v>
       </c>
       <c r="U6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V6" s="6"/>
+      <c r="V6" s="7"/>
       <c r="W6" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>ESCIVM</v>
       </c>
       <c r="X6" s="5" t="str">
-        <f t="shared" ref="X6" si="41">UPPER(X5)</f>
+        <f t="shared" ref="X6" si="43">UPPER(X5)</f>
         <v>NACIOM</v>
       </c>
       <c r="Y6" s="5" t="str">
-        <f t="shared" ref="Y6" si="42">UPPER(Y5)</f>
+        <f t="shared" ref="Y6" si="44">UPPER(Y5)</f>
         <v>ESCOLAM</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA6" s="6"/>
+      <c r="AA6" s="7"/>
       <c r="AB6" s="5" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>CAUDEF</v>
       </c>
       <c r="AC6" s="5" t="str">
-        <f t="shared" ref="AC6" si="43">UPPER(AC5)</f>
+        <f t="shared" ref="AC6" si="45">UPPER(AC5)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD6" s="5" t="str">
-        <f t="shared" ref="AD6" si="44">UPPER(AD5)</f>
+        <f t="shared" ref="AD6" si="46">UPPER(AD5)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE6" s="5" t="str">
-        <f t="shared" ref="AE6" si="45">UPPER(AE5)</f>
+        <f t="shared" ref="AE6" si="47">UPPER(AE5)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF6" s="5" t="str">
-        <f t="shared" ref="AF6" si="46">UPPER(AF5)</f>
+        <f t="shared" ref="AF6" si="48">UPPER(AF5)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG6" s="5" t="str">
-        <f t="shared" ref="AG6" si="47">UPPER(AG5)</f>
+        <f t="shared" ref="AG6" si="49">UPPER(AG5)</f>
         <v>TOHIVI</v>
       </c>
     </row>
@@ -1206,31 +1221,31 @@
         <v>31</v>
       </c>
       <c r="E7" s="5" t="str">
-        <f>UPPER(E6)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F7" s="5" t="str">
-        <f>UPPER(F6)</f>
+        <f t="shared" si="33"/>
         <v>DEPOCU</v>
       </c>
       <c r="G7" s="5" t="str">
-        <f t="shared" ref="G7" si="48">UPPER(G6)</f>
+        <f t="shared" ref="G7" si="50">UPPER(G6)</f>
         <v>MUPOCU</v>
       </c>
       <c r="H7" s="5" t="str">
-        <f t="shared" ref="H7" si="49">UPPER(H6)</f>
+        <f t="shared" ref="H7" si="51">UPPER(H6)</f>
         <v>AREAG</v>
       </c>
       <c r="I7" s="5" t="str">
-        <f t="shared" ref="I7" si="50">UPPER(I6)</f>
+        <f t="shared" ref="I7" si="52">UPPER(I6)</f>
         <v>SEXO</v>
       </c>
       <c r="J7" s="5" t="str">
-        <f t="shared" ref="J7" si="51">UPPER(J6)</f>
+        <f t="shared" ref="J7" si="53">UPPER(J6)</f>
         <v>DIAOCU</v>
       </c>
       <c r="K7" s="5" t="str">
-        <f t="shared" ref="K7" si="52">UPPER(K6)</f>
+        <f t="shared" ref="K7" si="54">UPPER(K6)</f>
         <v>MESOCU</v>
       </c>
       <c r="L7" s="5" t="str">
@@ -1241,19 +1256,19 @@
         <v>32</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f>UPPER(N6)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O7" s="5" t="str">
-        <f t="shared" ref="O7" si="53">UPPER(O6)</f>
+        <f t="shared" ref="O7" si="55">UPPER(O6)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P7" s="5" t="str">
-        <f t="shared" ref="P7" si="54">UPPER(P6)</f>
+        <f t="shared" ref="P7" si="56">UPPER(P6)</f>
         <v>SEMGES</v>
       </c>
       <c r="Q7" s="5" t="str">
-        <f t="shared" ref="Q7" si="55">UPPER(Q6)</f>
+        <f t="shared" ref="Q7" si="57">UPPER(Q6)</f>
         <v>EDADM</v>
       </c>
       <c r="R7" s="5" t="s">
@@ -1264,51 +1279,50 @@
         <v>DEPREM</v>
       </c>
       <c r="T7" s="5" t="str">
-        <f t="shared" ref="T7" si="56">UPPER(T6)</f>
+        <f t="shared" ref="T7" si="58">UPPER(T6)</f>
         <v>MUPREM</v>
       </c>
       <c r="U7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="6"/>
+      <c r="V7" s="7"/>
       <c r="W7" s="5" t="str">
-        <f t="shared" ref="W7" si="57">UPPER(W6)</f>
+        <f t="shared" ref="W7" si="59">UPPER(W6)</f>
         <v>ESCIVM</v>
       </c>
-      <c r="X7" s="5" t="str">
-        <f t="shared" ref="X7" si="58">UPPER(X6)</f>
-        <v>NACIOM</v>
+      <c r="X7" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="Y7" s="5" t="str">
-        <f t="shared" ref="Y7" si="59">UPPER(Y6)</f>
+        <f t="shared" ref="Y7" si="60">UPPER(Y6)</f>
         <v>ESCOLAM</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA7" s="6"/>
+      <c r="AA7" s="7"/>
       <c r="AB7" s="5" t="str">
-        <f t="shared" ref="AB7" si="60">UPPER(AB6)</f>
+        <f t="shared" ref="AB7" si="61">UPPER(AB6)</f>
         <v>CAUDEF</v>
       </c>
       <c r="AC7" s="5" t="str">
-        <f t="shared" ref="AC7" si="61">UPPER(AC6)</f>
+        <f t="shared" ref="AC7" si="62">UPPER(AC6)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD7" s="5" t="str">
-        <f t="shared" ref="AD7" si="62">UPPER(AD6)</f>
+        <f t="shared" ref="AD7" si="63">UPPER(AD6)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE7" s="5" t="str">
-        <f t="shared" ref="AE7" si="63">UPPER(AE6)</f>
+        <f t="shared" ref="AE7" si="64">UPPER(AE6)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF7" s="5" t="str">
-        <f t="shared" ref="AF7" si="64">UPPER(AF6)</f>
+        <f t="shared" ref="AF7" si="65">UPPER(AF6)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG7" s="5" t="str">
-        <f t="shared" ref="AG7" si="65">UPPER(AG6)</f>
+        <f t="shared" ref="AG7" si="66">UPPER(AG6)</f>
         <v>TOHIVI</v>
       </c>
     </row>
@@ -1326,31 +1340,31 @@
         <v>31</v>
       </c>
       <c r="E8" s="5" t="str">
-        <f>UPPER(E7)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F8" s="5" t="str">
-        <f>UPPER(F7)</f>
+        <f t="shared" si="33"/>
         <v>DEPOCU</v>
       </c>
       <c r="G8" s="5" t="str">
-        <f t="shared" ref="G8" si="66">UPPER(G7)</f>
+        <f t="shared" ref="G8" si="67">UPPER(G7)</f>
         <v>MUPOCU</v>
       </c>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8" si="67">UPPER(H7)</f>
+        <f t="shared" ref="H8" si="68">UPPER(H7)</f>
         <v>AREAG</v>
       </c>
       <c r="I8" s="5" t="str">
-        <f>UPPER(I7)</f>
+        <f t="shared" ref="I8:K11" si="69">UPPER(I7)</f>
         <v>SEXO</v>
       </c>
       <c r="J8" s="5" t="str">
-        <f>UPPER(J7)</f>
+        <f t="shared" si="69"/>
         <v>DIAOCU</v>
       </c>
       <c r="K8" s="5" t="str">
-        <f>UPPER(K7)</f>
+        <f t="shared" si="69"/>
         <v>MESOCU</v>
       </c>
       <c r="L8" s="5" t="s">
@@ -1360,19 +1374,19 @@
         <v>32</v>
       </c>
       <c r="N8" s="5" t="str">
-        <f>UPPER(N7)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O8" s="5" t="str">
-        <f t="shared" ref="O8" si="68">UPPER(O7)</f>
+        <f t="shared" ref="O8" si="70">UPPER(O7)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P8" s="5" t="str">
-        <f t="shared" ref="P8" si="69">UPPER(P7)</f>
+        <f t="shared" ref="P8" si="71">UPPER(P7)</f>
         <v>SEMGES</v>
       </c>
       <c r="Q8" s="5" t="str">
-        <f t="shared" ref="Q8" si="70">UPPER(Q7)</f>
+        <f t="shared" ref="Q8" si="72">UPPER(Q7)</f>
         <v>EDADM</v>
       </c>
       <c r="R8" s="5" t="s">
@@ -1387,45 +1401,44 @@
       <c r="U8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V8" s="6"/>
+      <c r="V8" s="7"/>
       <c r="W8" s="5" t="str">
-        <f t="shared" ref="W8" si="71">UPPER(W7)</f>
+        <f t="shared" ref="W8" si="73">UPPER(W7)</f>
         <v>ESCIVM</v>
       </c>
-      <c r="X8" s="5" t="str">
-        <f t="shared" ref="X8" si="72">UPPER(X7)</f>
-        <v>NACIOM</v>
+      <c r="X8" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="Y8" s="5" t="str">
-        <f t="shared" ref="Y8" si="73">UPPER(Y7)</f>
+        <f t="shared" ref="Y8" si="74">UPPER(Y7)</f>
         <v>ESCOLAM</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA8" s="6"/>
+      <c r="AA8" s="7"/>
       <c r="AB8" s="5" t="str">
-        <f t="shared" ref="AB8" si="74">UPPER(AB7)</f>
+        <f t="shared" ref="AB8" si="75">UPPER(AB7)</f>
         <v>CAUDEF</v>
       </c>
       <c r="AC8" s="5" t="str">
-        <f t="shared" ref="AC8" si="75">UPPER(AC7)</f>
+        <f t="shared" ref="AC8" si="76">UPPER(AC7)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD8" s="5" t="str">
-        <f t="shared" ref="AD8" si="76">UPPER(AD7)</f>
+        <f t="shared" ref="AD8" si="77">UPPER(AD7)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE8" s="5" t="str">
-        <f t="shared" ref="AE8" si="77">UPPER(AE7)</f>
+        <f t="shared" ref="AE8" si="78">UPPER(AE7)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF8" s="5" t="str">
-        <f t="shared" ref="AF8" si="78">UPPER(AF7)</f>
+        <f t="shared" ref="AF8" si="79">UPPER(AF7)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG8" s="5" t="str">
-        <f t="shared" ref="AG8" si="79">UPPER(AG7)</f>
+        <f t="shared" ref="AG8" si="80">UPPER(AG7)</f>
         <v>TOHIVI</v>
       </c>
     </row>
@@ -1443,31 +1456,31 @@
         <v>31</v>
       </c>
       <c r="E9" s="5" t="str">
-        <f>UPPER(E8)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F9" s="5" t="str">
-        <f>UPPER(F8)</f>
+        <f t="shared" si="33"/>
         <v>DEPOCU</v>
       </c>
       <c r="G9" s="5" t="str">
-        <f t="shared" ref="G9" si="80">UPPER(G8)</f>
+        <f t="shared" ref="G9" si="81">UPPER(G8)</f>
         <v>MUPOCU</v>
       </c>
       <c r="H9" s="5" t="str">
-        <f t="shared" ref="H9" si="81">UPPER(H8)</f>
+        <f t="shared" ref="H9" si="82">UPPER(H8)</f>
         <v>AREAG</v>
       </c>
       <c r="I9" s="5" t="str">
-        <f>UPPER(I8)</f>
+        <f t="shared" si="69"/>
         <v>SEXO</v>
       </c>
       <c r="J9" s="5" t="str">
-        <f>UPPER(J8)</f>
+        <f t="shared" si="69"/>
         <v>DIAOCU</v>
       </c>
       <c r="K9" s="5" t="str">
-        <f>UPPER(K8)</f>
+        <f t="shared" si="69"/>
         <v>MESOCU</v>
       </c>
       <c r="L9" s="5" t="s">
@@ -1477,19 +1490,19 @@
         <v>32</v>
       </c>
       <c r="N9" s="5" t="str">
-        <f>UPPER(N8)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O9" s="5" t="str">
-        <f t="shared" ref="O9" si="82">UPPER(O8)</f>
+        <f t="shared" ref="O9" si="83">UPPER(O8)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P9" s="5" t="str">
-        <f t="shared" ref="P9" si="83">UPPER(P8)</f>
+        <f t="shared" ref="P9" si="84">UPPER(P8)</f>
         <v>SEMGES</v>
       </c>
       <c r="Q9" s="5" t="str">
-        <f t="shared" ref="Q9" si="84">UPPER(Q8)</f>
+        <f t="shared" ref="Q9" si="85">UPPER(Q8)</f>
         <v>EDADM</v>
       </c>
       <c r="R9" s="5" t="s">
@@ -1504,14 +1517,13 @@
       <c r="U9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V9" s="6"/>
+      <c r="V9" s="7"/>
       <c r="W9" s="5" t="str">
-        <f t="shared" ref="W9" si="85">UPPER(W8)</f>
+        <f t="shared" ref="W9" si="86">UPPER(W8)</f>
         <v>ESCIVM</v>
       </c>
-      <c r="X9" s="5" t="str">
-        <f t="shared" ref="X9" si="86">UPPER(X8)</f>
-        <v>NACIOM</v>
+      <c r="X9" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="Y9" s="5" t="str">
         <f t="shared" ref="Y9" si="87">UPPER(Y8)</f>
@@ -1520,7 +1532,7 @@
       <c r="Z9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA9" s="6"/>
+      <c r="AA9" s="7"/>
       <c r="AB9" s="5" t="str">
         <f t="shared" ref="AB9" si="88">UPPER(AB8)</f>
         <v>CAUDEF</v>
@@ -1560,28 +1572,28 @@
         <v>31</v>
       </c>
       <c r="E10" s="5" t="str">
-        <f>UPPER(E9)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F10" s="5" t="str">
-        <f>UPPER(F9)</f>
+        <f t="shared" si="33"/>
         <v>DEPOCU</v>
       </c>
       <c r="G10" s="5" t="str">
         <f t="shared" ref="G10" si="94">UPPER(G9)</f>
         <v>MUPOCU</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="5" t="str">
-        <f>UPPER(I9)</f>
+        <f t="shared" si="69"/>
         <v>SEXO</v>
       </c>
       <c r="J10" s="5" t="str">
-        <f>UPPER(J9)</f>
+        <f t="shared" si="69"/>
         <v>DIAOCU</v>
       </c>
       <c r="K10" s="5" t="str">
-        <f>UPPER(K9)</f>
+        <f t="shared" si="69"/>
         <v>MESOCU</v>
       </c>
       <c r="L10" s="5" t="s">
@@ -1591,7 +1603,7 @@
         <v>32</v>
       </c>
       <c r="N10" s="5" t="str">
-        <f>UPPER(N9)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O10" s="5" t="str">
@@ -1618,41 +1630,40 @@
       <c r="U10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="6"/>
+      <c r="V10" s="7"/>
       <c r="W10" s="5" t="str">
         <f t="shared" ref="W10" si="98">UPPER(W9)</f>
         <v>ESCIVM</v>
       </c>
-      <c r="X10" s="5" t="str">
-        <f t="shared" ref="X10" si="99">UPPER(X9)</f>
-        <v>NACIOM</v>
+      <c r="X10" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="Y10" s="5" t="str">
-        <f t="shared" ref="Y10" si="100">UPPER(Y9)</f>
+        <f t="shared" ref="Y10" si="99">UPPER(Y9)</f>
         <v>ESCOLAM</v>
       </c>
       <c r="Z10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA10" s="6"/>
+      <c r="AA10" s="7"/>
       <c r="AB10" s="5" t="str">
-        <f t="shared" ref="AB10" si="101">UPPER(AB9)</f>
+        <f t="shared" ref="AB10" si="100">UPPER(AB9)</f>
         <v>CAUDEF</v>
       </c>
       <c r="AC10" s="5" t="str">
-        <f t="shared" ref="AC10" si="102">UPPER(AC9)</f>
+        <f t="shared" ref="AC10" si="101">UPPER(AC9)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD10" s="5" t="str">
-        <f t="shared" ref="AD10" si="103">UPPER(AD9)</f>
+        <f t="shared" ref="AD10" si="102">UPPER(AD9)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE10" s="5" t="str">
-        <f t="shared" ref="AE10" si="104">UPPER(AE9)</f>
+        <f t="shared" ref="AE10" si="103">UPPER(AE9)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF10" s="5" t="str">
-        <f t="shared" ref="AF10" si="105">UPPER(AF9)</f>
+        <f t="shared" ref="AF10" si="104">UPPER(AF9)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG10" s="5" t="str">
@@ -1674,28 +1685,28 @@
         <v>31</v>
       </c>
       <c r="E11" s="5" t="str">
-        <f>UPPER(E10)</f>
+        <f t="shared" si="0"/>
         <v>AÑOREG</v>
       </c>
       <c r="F11" s="5" t="str">
-        <f>UPPER(F10)</f>
+        <f t="shared" si="33"/>
         <v>DEPOCU</v>
       </c>
       <c r="G11" s="5" t="str">
-        <f t="shared" ref="G11" si="106">UPPER(G10)</f>
+        <f t="shared" ref="G11" si="105">UPPER(G10)</f>
         <v>MUPOCU</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="5" t="str">
-        <f>UPPER(I10)</f>
+        <f t="shared" si="69"/>
         <v>SEXO</v>
       </c>
       <c r="J11" s="5" t="str">
-        <f>UPPER(J10)</f>
+        <f t="shared" si="69"/>
         <v>DIAOCU</v>
       </c>
       <c r="K11" s="5" t="str">
-        <f>UPPER(K10)</f>
+        <f t="shared" si="69"/>
         <v>MESOCU</v>
       </c>
       <c r="L11" s="5" t="s">
@@ -1705,19 +1716,19 @@
         <v>32</v>
       </c>
       <c r="N11" s="5" t="str">
-        <f>UPPER(N10)</f>
+        <f t="shared" si="5"/>
         <v>CLAPAR</v>
       </c>
       <c r="O11" s="5" t="str">
-        <f t="shared" ref="O11" si="107">UPPER(O10)</f>
+        <f t="shared" ref="O11" si="106">UPPER(O10)</f>
         <v>VIAPAR</v>
       </c>
       <c r="P11" s="5" t="str">
-        <f t="shared" ref="P11" si="108">UPPER(P10)</f>
+        <f t="shared" ref="P11" si="107">UPPER(P10)</f>
         <v>SEMGES</v>
       </c>
       <c r="Q11" s="5" t="str">
-        <f t="shared" ref="Q11" si="109">UPPER(Q10)</f>
+        <f t="shared" ref="Q11" si="108">UPPER(Q10)</f>
         <v>EDADM</v>
       </c>
       <c r="R11" s="5" t="s">
@@ -1732,41 +1743,40 @@
       <c r="U11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V11" s="6"/>
+      <c r="V11" s="7"/>
       <c r="W11" s="5" t="str">
-        <f t="shared" ref="W11" si="110">UPPER(W10)</f>
+        <f t="shared" ref="W11" si="109">UPPER(W10)</f>
         <v>ESCIVM</v>
       </c>
-      <c r="X11" s="5" t="str">
-        <f t="shared" ref="X11" si="111">UPPER(X10)</f>
-        <v>NACIOM</v>
+      <c r="X11" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="Y11" s="5" t="str">
-        <f t="shared" ref="Y11" si="112">UPPER(Y10)</f>
+        <f t="shared" ref="Y11" si="110">UPPER(Y10)</f>
         <v>ESCOLAM</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA11" s="6"/>
+      <c r="AA11" s="7"/>
       <c r="AB11" s="5" t="str">
-        <f t="shared" ref="AB11" si="113">UPPER(AB10)</f>
+        <f t="shared" ref="AB11" si="111">UPPER(AB10)</f>
         <v>CAUDEF</v>
       </c>
       <c r="AC11" s="5" t="str">
-        <f t="shared" ref="AC11" si="114">UPPER(AC10)</f>
+        <f t="shared" ref="AC11" si="112">UPPER(AC10)</f>
         <v>ASISREC</v>
       </c>
       <c r="AD11" s="5" t="str">
-        <f t="shared" ref="AD11" si="115">UPPER(AD10)</f>
+        <f t="shared" ref="AD11" si="113">UPPER(AD10)</f>
         <v>SITIOOCU</v>
       </c>
       <c r="AE11" s="5" t="str">
-        <f t="shared" ref="AE11" si="116">UPPER(AE10)</f>
+        <f t="shared" ref="AE11" si="114">UPPER(AE10)</f>
         <v>TOHITE</v>
       </c>
       <c r="AF11" s="5" t="str">
-        <f t="shared" ref="AF11" si="117">UPPER(AF10)</f>
+        <f t="shared" ref="AF11" si="115">UPPER(AF10)</f>
         <v>TOHINM</v>
       </c>
       <c r="AG11" s="5" t="str">
@@ -2007,7 +2017,104 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
+      <c r="A42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>